<commit_message>
Fix test RAD 471 e 472
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.57/report-checklist.xlsx
+++ b/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.57/report-checklist.xlsx
@@ -2662,22 +2662,22 @@
       </c>
       <c r="F10" s="78" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G10" s="78" t="inlineStr">
         <is>
-          <t>2025-12-18T10:52:06Z</t>
+          <t>2025-12-30T11:16:12Z</t>
         </is>
       </c>
       <c r="H10" s="78" t="inlineStr">
         <is>
-          <t>d0e63b23fa6b0e26bb00470d89ace59f</t>
+          <t>2edbd04af1ef17891a14390599d6ce92</t>
         </is>
       </c>
       <c r="I10" s="79" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.80d1b1c6668071368ff8e999748bc5f4dca9c24fdf18fc43af785ead29c43d97.798b33a24d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.f45c8971f08a67ad076f21faa34ecc1b299a8b531bdd2e08fc95959d7bc32992.da0889374f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J10" s="80" t="inlineStr">
@@ -3088,12 +3088,12 @@
       </c>
       <c r="F17" s="88" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G17" s="88" t="inlineStr">
         <is>
-          <t>2025-12-19T15:30:17Z</t>
+          <t>2025-12-30T11:17:26Z</t>
         </is>
       </c>
       <c r="H17" s="88" t="inlineStr">
@@ -3192,12 +3192,12 @@
       </c>
       <c r="F18" s="88" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G18" s="88" t="inlineStr">
         <is>
-          <t>2025-12-19T15:30:17Z</t>
+          <t>2025-12-30T11:17:26Z</t>
         </is>
       </c>
       <c r="H18" s="88" t="inlineStr">
@@ -3296,12 +3296,12 @@
       </c>
       <c r="F19" s="88" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G19" s="88" t="inlineStr">
         <is>
-          <t>2025-12-19T15:30:17Z</t>
+          <t>2025-12-30T11:17:26Z</t>
         </is>
       </c>
       <c r="H19" s="88" t="inlineStr">
@@ -5585,22 +5585,22 @@
       </c>
       <c r="F59" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G59" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18T10:52:13Z</t>
+          <t>2025-12-30T11:16:19Z</t>
         </is>
       </c>
       <c r="H59" s="79" t="inlineStr">
         <is>
-          <t>f3f5e350ac1a1079bb8cdb05f4b62b33</t>
+          <t>30ef7e9f50574ddb454be5d3ca7024e8</t>
         </is>
       </c>
       <c r="I59" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.a03ee56f6c19bf59d6b73354a4cda0cca0d289f8e50781c3106103d7c72e0db2.0f2b05df9c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.be36f55d4c207f7656a58fee544f1de430554674e0855df05f095d894857f12f.df9f4a2a83^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J59" s="80" t="inlineStr">
@@ -5658,22 +5658,22 @@
       </c>
       <c r="F60" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G60" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18T10:52:13Z</t>
+          <t>2025-12-30T11:16:19Z</t>
         </is>
       </c>
       <c r="H60" s="79" t="inlineStr">
         <is>
-          <t>34e7a8e065506b9cbe10d3415841712d</t>
+          <t>f596a6a1698d86f3b4046cd435abdafa</t>
         </is>
       </c>
       <c r="I60" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.4f597e907bf4dbdf8421a867c85c98a803d7b3df3e6a283f15edd0868fd9f0b8.55a3e88a2f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.c3bf9c71bbc51c21d755e95b93e1d062a1712253d51a52b4a7780551f37ec59e.b60fbe6373^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J60" s="80" t="inlineStr">
@@ -5730,22 +5730,22 @@
       </c>
       <c r="F61" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G61" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18T10:53:05Z</t>
+          <t>2025-12-30T11:17:11Z</t>
         </is>
       </c>
       <c r="H61" s="79" t="inlineStr">
         <is>
-          <t>5255f3ad8df984ab1f9ff0f66ad364cc</t>
+          <t>5050638616db87a1d6c41c70978ab4e3</t>
         </is>
       </c>
       <c r="I61" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.632576c3508487ca9d9d488d0f241f7c15cd95e3053141de9454f5e7028fc1b6.82f4427c01^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.e0f1c1ad53c560ef99f815eba049cff019a72eb67b6247b769d1f875c5c05088.762d7579ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J61" s="80" t="inlineStr">
@@ -5802,22 +5802,22 @@
       </c>
       <c r="F62" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G62" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18T10:53:09Z</t>
+          <t>2025-12-30T11:17:15Z</t>
         </is>
       </c>
       <c r="H62" s="79" t="inlineStr">
         <is>
-          <t>f813ad4bff312c6fea791c582fafdf4f</t>
+          <t>e17c12b027143c761ff766d757d59c11</t>
         </is>
       </c>
       <c r="I62" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.ac2711301b2f06029955b375f528261c0eb476e36cd148eeab4b3a8691d08b7f.616e6c433c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.d6bfedcee49ef5064aa6b8506525b2674f9b180a60f0f466d061cbe47e418500.89cad54e18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J62" s="80" t="inlineStr">
@@ -5875,22 +5875,22 @@
       </c>
       <c r="F63" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G63" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18T10:52:09Z</t>
+          <t>2025-12-30T11:16:15Z</t>
         </is>
       </c>
       <c r="H63" s="79" t="inlineStr">
         <is>
-          <t>22ae828e339fe3e035193db3f884bc3a</t>
+          <t>5d64c74afc5d02afc57342f087c609b6</t>
         </is>
       </c>
       <c r="I63" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.0873b387aa7c198a8eef05191c698abc2dcaf15207026e6bceed41efd42ce70f.6972a2e6af^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.9e4f2b11d6545b4fd91ba8941a2d480268855c5d74a28c89e1b2cdee11bb860b.54f23a041d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J63" s="80" t="inlineStr">
@@ -6171,22 +6171,22 @@
       </c>
       <c r="F68" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G68" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18T10:53:12Z</t>
+          <t>2025-12-30T11:17:18Z</t>
         </is>
       </c>
       <c r="H68" s="79" t="inlineStr">
         <is>
-          <t>5351cf333888a3178e4b22d4cf62c40e</t>
+          <t>61226a8bf5de4a2a56ebc79552e1eb4f</t>
         </is>
       </c>
       <c r="I68" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.f9d9a42e7fba5710ea14334b51c61e60b916295f874256778b1dc1d62d7bd5a4.a4c8adfb37^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.0836d3aac2a8f52de744c6c52898c249a80186456a0377796ca0d30381cda089.28bd19b905^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J68" s="80" t="inlineStr">
@@ -6243,22 +6243,22 @@
       </c>
       <c r="F69" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="G69" s="79" t="inlineStr">
         <is>
-          <t>2025-12-18T10:53:16Z</t>
+          <t>2025-12-30T11:17:22Z</t>
         </is>
       </c>
       <c r="H69" s="79" t="inlineStr">
         <is>
-          <t>3179acd23daca90c0553fe9c2ff92b2f</t>
+          <t>f128ae1fa35ea2aafce17c0d749ee3f8</t>
         </is>
       </c>
       <c r="I69" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.18360b12943cec1d265c6fe5ae798ab1ca5fef720de0141a26c36d8783622dc7.fd1181b51d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.d3b184077e36c1cedf14dfb6f6722a83578d296ed46e1a71e129c522f5c14931.94fc46486d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J69" s="80" t="inlineStr">

</xml_diff>

<commit_message>
Fix test RAD 472
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.57/report-checklist.xlsx
+++ b/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.57/report-checklist.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="33720" yWindow="975" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Istruzioni Compilazione" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Prerequisiti" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TestCases" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="LISTA VALORI" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="Summary" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Istruzioni Compilazione" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Prerequisiti" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestCases" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LISTA VALORI" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'TestCases'!$A$9:$W$190</definedName>
@@ -2662,22 +2662,22 @@
       </c>
       <c r="F10" s="78" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G10" s="78" t="inlineStr">
         <is>
-          <t>2025-12-30T11:16:12Z</t>
+          <t>2026-01-09T14:14:29Z</t>
         </is>
       </c>
       <c r="H10" s="78" t="inlineStr">
         <is>
-          <t>2edbd04af1ef17891a14390599d6ce92</t>
+          <t>c58b4a2db4d497a01144cc96906f0b49</t>
         </is>
       </c>
       <c r="I10" s="79" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.f45c8971f08a67ad076f21faa34ecc1b299a8b531bdd2e08fc95959d7bc32992.da0889374f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.73cdef8a51e40894f00bd902cc5f7a8bd08802da8f35bbeafe7da4f2b00424ce.bfa6cd8fbf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J10" s="80" t="inlineStr">
@@ -3088,12 +3088,12 @@
       </c>
       <c r="F17" s="88" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G17" s="88" t="inlineStr">
         <is>
-          <t>2025-12-30T11:17:26Z</t>
+          <t>2026-01-09T14:15:45Z</t>
         </is>
       </c>
       <c r="H17" s="88" t="inlineStr">
@@ -3192,12 +3192,12 @@
       </c>
       <c r="F18" s="88" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G18" s="88" t="inlineStr">
         <is>
-          <t>2025-12-30T11:17:26Z</t>
+          <t>2026-01-09T14:15:45Z</t>
         </is>
       </c>
       <c r="H18" s="88" t="inlineStr">
@@ -3296,12 +3296,12 @@
       </c>
       <c r="F19" s="88" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G19" s="88" t="inlineStr">
         <is>
-          <t>2025-12-30T11:17:26Z</t>
+          <t>2026-01-09T14:15:45Z</t>
         </is>
       </c>
       <c r="H19" s="88" t="inlineStr">
@@ -5585,22 +5585,22 @@
       </c>
       <c r="F59" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G59" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30T11:16:19Z</t>
+          <t>2026-01-09T14:14:36Z</t>
         </is>
       </c>
       <c r="H59" s="79" t="inlineStr">
         <is>
-          <t>30ef7e9f50574ddb454be5d3ca7024e8</t>
+          <t>65ab976e9426a9c869537ef94f16d359</t>
         </is>
       </c>
       <c r="I59" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.be36f55d4c207f7656a58fee544f1de430554674e0855df05f095d894857f12f.df9f4a2a83^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.b4292d787ead7831b28c9ebe0aba06d546315c3def58c8fc89f15e2ef00e3422.4e9caf6752^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J59" s="80" t="inlineStr">
@@ -5658,22 +5658,22 @@
       </c>
       <c r="F60" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G60" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30T11:16:19Z</t>
+          <t>2026-01-09T14:14:37Z</t>
         </is>
       </c>
       <c r="H60" s="79" t="inlineStr">
         <is>
-          <t>f596a6a1698d86f3b4046cd435abdafa</t>
+          <t>0c48d0d88c747e9b1bfdbd5075de333e</t>
         </is>
       </c>
       <c r="I60" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.c3bf9c71bbc51c21d755e95b93e1d062a1712253d51a52b4a7780551f37ec59e.b60fbe6373^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.a202d39cf94e36375838aed735e962107883963e0c3b25b821384840b79e3cbf.1f9d0f9331^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J60" s="80" t="inlineStr">
@@ -5730,22 +5730,22 @@
       </c>
       <c r="F61" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G61" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30T11:17:11Z</t>
+          <t>2026-01-09T14:15:29Z</t>
         </is>
       </c>
       <c r="H61" s="79" t="inlineStr">
         <is>
-          <t>5050638616db87a1d6c41c70978ab4e3</t>
+          <t>7bfd208491058c08f636ff6f4e7b5605</t>
         </is>
       </c>
       <c r="I61" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.e0f1c1ad53c560ef99f815eba049cff019a72eb67b6247b769d1f875c5c05088.762d7579ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.8b4a284ff4bd60a74df68bdc32038fa8dcbdd9923f338fae83cb3066e8867033.d2efc7c996^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J61" s="80" t="inlineStr">
@@ -5802,22 +5802,22 @@
       </c>
       <c r="F62" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G62" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30T11:17:15Z</t>
+          <t>2026-01-09T14:15:33Z</t>
         </is>
       </c>
       <c r="H62" s="79" t="inlineStr">
         <is>
-          <t>e17c12b027143c761ff766d757d59c11</t>
+          <t>6d724025cff0478c06b88da34d73e5d5</t>
         </is>
       </c>
       <c r="I62" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.d6bfedcee49ef5064aa6b8506525b2674f9b180a60f0f466d061cbe47e418500.89cad54e18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.efe34371a1f874e037660edfdec89a2a9e03bf59748a3988ff199a0fa6314f3d.0e8949d413^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J62" s="80" t="inlineStr">
@@ -5875,22 +5875,22 @@
       </c>
       <c r="F63" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G63" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30T11:16:15Z</t>
+          <t>2026-01-09T14:14:33Z</t>
         </is>
       </c>
       <c r="H63" s="79" t="inlineStr">
         <is>
-          <t>5d64c74afc5d02afc57342f087c609b6</t>
+          <t>94d405dbb4125cc2922b57a1b27a0c77</t>
         </is>
       </c>
       <c r="I63" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.9e4f2b11d6545b4fd91ba8941a2d480268855c5d74a28c89e1b2cdee11bb860b.54f23a041d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.673f1ea3a6144f965d6dee65005fb1b6e4c02e11e726ddc5d73ec427996c14de.90c2f32dc7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J63" s="80" t="inlineStr">
@@ -6171,22 +6171,22 @@
       </c>
       <c r="F68" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G68" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30T11:17:18Z</t>
+          <t>2026-01-09T14:15:37Z</t>
         </is>
       </c>
       <c r="H68" s="79" t="inlineStr">
         <is>
-          <t>61226a8bf5de4a2a56ebc79552e1eb4f</t>
+          <t>b95cf214485a328617f171af0734e0a2</t>
         </is>
       </c>
       <c r="I68" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.0836d3aac2a8f52de744c6c52898c249a80186456a0377796ca0d30381cda089.28bd19b905^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.747f47419628f62ede6088c48e37ab65d15b6b843c36c9694fc6017f2f72d7af.df927bb17b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J68" s="80" t="inlineStr">
@@ -6243,22 +6243,22 @@
       </c>
       <c r="F69" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="G69" s="79" t="inlineStr">
         <is>
-          <t>2025-12-30T11:17:22Z</t>
+          <t>2026-01-09T14:15:40Z</t>
         </is>
       </c>
       <c r="H69" s="79" t="inlineStr">
         <is>
-          <t>f128ae1fa35ea2aafce17c0d749ee3f8</t>
+          <t>9a751c1b660643034b089e81a05b1e0d</t>
         </is>
       </c>
       <c r="I69" s="93" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.d3b184077e36c1cedf14dfb6f6722a83578d296ed46e1a71e129c522f5c14931.94fc46486d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.6783b6242a52865e28d78769ffea9b4154b82cbe90b589e5f61e369341f752d9.5b6b8a8ada^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J69" s="80" t="inlineStr">

</xml_diff>